<commit_message>
Add more linkedin code
</commit_message>
<xml_diff>
--- a/company/linkedin/linkedin高频.xlsx
+++ b/company/linkedin/linkedin高频.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bozhou/Dropbox/interview/company/linkedin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96BDA29-D983-EB4F-BABB-3A7EF1B0043C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B226ED1D-B97F-C34A-92E8-47C3353B874C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="73440" yWindow="3580" windowWidth="28040" windowHeight="17440" xr2:uid="{04ABC891-5ECD-B14B-BBD8-A93D32370AA1}"/>
+    <workbookView xWindow="75240" yWindow="3700" windowWidth="28040" windowHeight="17440" xr2:uid="{04ABC891-5ECD-B14B-BBD8-A93D32370AA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -649,7 +649,7 @@
   <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update code and add more company questions
</commit_message>
<xml_diff>
--- a/company/linkedin/linkedin高频.xlsx
+++ b/company/linkedin/linkedin高频.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bozhou/Dropbox/interview/company/linkedin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DBB536-9949-234E-A9DD-6A6A9F56435C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FFCD2B-15D8-EC48-AEC4-54529743BF1D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51180" yWindow="4100" windowWidth="17420" windowHeight="17440" xr2:uid="{04ABC891-5ECD-B14B-BBD8-A93D32370AA1}"/>
+    <workbookView xWindow="72400" yWindow="4000" windowWidth="17420" windowHeight="17440" activeTab="1" xr2:uid="{04ABC891-5ECD-B14B-BBD8-A93D32370AA1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Algorithm" sheetId="1" r:id="rId1"/>
+    <sheet name="Design" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="128">
   <si>
     <t>Leetcode number</t>
   </si>
@@ -319,6 +320,102 @@
   </si>
   <si>
     <t>Same Tree</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Freq</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>shorten url的各‍‌‌‍‍‍‌‌‌‌‌‌‍‍种变种，比如新添feature：click stats，就是统计每个short url被read多少次</t>
+  </si>
+  <si>
+    <t>设计一个K/V store，支持基于单个KEY的insert/update/delete/fetch 操作，基本上照着RocksDB/Couchbase的实现来聊的</t>
+  </si>
+  <si>
+    <t>设计一个metric系统，包括怎么收集，aggregation，存储，查询，dashboard，alert</t>
+  </si>
+  <si>
+    <t>design monitoring system</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-542321-1-1.html</t>
+  </si>
+  <si>
+    <t>Design top k exception in 24 hours.</t>
+  </si>
+  <si>
+    <t>设计日历</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-532557-1-1.html</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-531929-1-1.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.1point3acres.com/bbs/thread-531528-1-1.html </t>
+  </si>
+  <si>
+    <t>设计一个全球范围内的blacklist service</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-531259-1-1.html</t>
+  </si>
+  <si>
+    <t>设计distributed Logging System</t>
+  </si>
+  <si>
+    <t>设计一个基于内存的streaming系统，stream以(timestamp‍‌‌‍‍‍‌‌‌‌‌‌‍‍, binary_size)的消息进入，然后client会query以ts结束大小为k的内容。</t>
+  </si>
+  <si>
+    <t>存储在线用户的在网站上的活动</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-520850-1-1.html</t>
+  </si>
+  <si>
+    <t>Delayed Task Scheduler</t>
+  </si>
+  <si>
+    <t>设计一个系统监督和管理领英第三方API的流量</t>
+  </si>
+  <si>
+    <t>设计一个诊断系统，类似地理说的Kafka加上ag‍‌‌‍‍‍‌‌‌‌‌‌‍‍gregator的设计方式</t>
+  </si>
+  <si>
+    <t>设计二级好友三级好友</t>
+  </si>
+  <si>
+    <t>Amazon Product Page. 分析表之间的关系</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-495284-1-1.html</t>
+  </si>
+  <si>
+    <t>Design Hangman Game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.1point3acres.com/bbs/thread-492225-1-1.html </t>
+  </si>
+  <si>
+    <t>设计trending linkedin share post</t>
+  </si>
+  <si>
+    <t>value体积比较大需要放在硬盘里面 另外随机写到硬盘会比较慢所以assume你要appending only</t>
+  </si>
+  <si>
+    <t>document repository</t>
+  </si>
+  <si>
+    <t>https://soulmachine.gitbooks.io/system-design/cn/task-scheduler.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.1point3acres.com/bbs/thread-446923-1-1.html </t>
   </si>
 </sst>
 </file>
@@ -751,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13919B8-F934-B64B-811A-4EC5AB312C98}">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1422,14 +1519,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B62" t="s">
+    <row r="62" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="9">
         <v>3</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D62" s="11" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1704,4 +1801,224 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6A42AC-6C29-7E41-9C84-E5ED64CCDD94}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="52.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{B880D39A-EB29-3B45-9D2E-C674DD1FEE92}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{7A6C955A-C9CB-D94E-9E47-1DFC63B4A29F}"/>
+    <hyperlink ref="C7" r:id="rId3" xr:uid="{CA4C8AD1-0DAF-1A43-A4AD-1D680D5EAA90}"/>
+    <hyperlink ref="C8" r:id="rId4" xr:uid="{607FD3F5-3481-2246-AA80-CADADE3D14E8}"/>
+    <hyperlink ref="C9" r:id="rId5" xr:uid="{D3CDFB96-9B44-B04D-A3A0-2F2823EAAE0C}"/>
+    <hyperlink ref="C13" r:id="rId6" xr:uid="{88AFD75B-027F-8748-884F-1743ABEE3E38}"/>
+    <hyperlink ref="C3" r:id="rId7" xr:uid="{157BEC7A-C7BA-3E40-9B5F-842A1E9241EB}"/>
+    <hyperlink ref="C4" r:id="rId8" xr:uid="{B149A8E5-D207-0042-9256-C5A6C5B35876}"/>
+    <hyperlink ref="C14" r:id="rId9" xr:uid="{F394E03C-7A35-014C-BB43-19BC16808AC8}"/>
+    <hyperlink ref="A2" r:id="rId10" xr:uid="{23CD15E4-7ED0-6047-B129-3A0760268310}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>